<commit_message>
@kulasekaran pay slip download is 80% completed and pay slip mail send screen is 70% completed
</commit_message>
<xml_diff>
--- a/payslipsystem/webroot/templates/pay_slip_template.xlsx
+++ b/payslipsystem/webroot/templates/pay_slip_template.xlsx
@@ -7,12 +7,10 @@
     <workbookView xWindow="240" yWindow="45" windowWidth="20055" windowHeight="7995"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="salary_pay_slip" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$N$40</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">salary_pay_slip!$A$1:$N$40</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
@@ -93,7 +91,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+  <numFmts count="2">
+    <numFmt numFmtId="178" formatCode="#,##0.0;[Red]#,##0.0"/>
+    <numFmt numFmtId="180" formatCode="0;[Red]0"/>
+  </numFmts>
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,12 +113,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="14"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
@@ -144,7 +140,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -251,101 +247,131 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -650,251 +676,253 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="D6" s="4"/>
+      <c r="E6" s="5"/>
+      <c r="K6" s="3" t="s">
         <v>4</v>
       </c>
+      <c r="L6" s="5"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="B8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="10" spans="1:19">
-      <c r="B10" s="1" t="s">
+      <c r="C10" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:19">
-      <c r="J11" s="2"/>
+      <c r="J11" s="7"/>
     </row>
     <row r="12" spans="1:19">
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="11" t="s">
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="13"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="10"/>
     </row>
     <row r="13" spans="1:19">
-      <c r="C13" s="14"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="16"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="13"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="C14" s="17" t="s">
+      <c r="C14" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="18"/>
-      <c r="E14" s="19"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="17"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="17" t="s">
+      <c r="G14" s="18"/>
+      <c r="H14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="18"/>
-      <c r="J14" s="19"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="16"/>
       <c r="K14" s="17"/>
-      <c r="L14" s="19"/>
+      <c r="L14" s="18"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="18"/>
-      <c r="E15" s="19"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="16"/>
       <c r="F15" s="17"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="17" t="s">
+      <c r="G15" s="18"/>
+      <c r="H15" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="18"/>
-      <c r="J15" s="19"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="16"/>
       <c r="K15" s="17"/>
-      <c r="L15" s="19"/>
+      <c r="L15" s="18"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="18"/>
-      <c r="E16" s="19"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="16"/>
       <c r="F16" s="17"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="17" t="s">
+      <c r="G16" s="18"/>
+      <c r="H16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="18"/>
-      <c r="J16" s="19"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="16"/>
       <c r="K16" s="17"/>
-      <c r="L16" s="19"/>
+      <c r="L16" s="18"/>
     </row>
     <row r="17" spans="3:12">
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="18"/>
-      <c r="E17" s="19"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="17"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="18"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="19"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="16"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="16"/>
     </row>
     <row r="18" spans="3:12">
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="17"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="21"/>
     </row>
     <row r="19" spans="3:12">
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="18"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="17"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="17" t="s">
+      <c r="D19" s="23"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="18"/>
-      <c r="J19" s="19"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="16"/>
       <c r="K19" s="17"/>
-      <c r="L19" s="19"/>
+      <c r="L19" s="18"/>
     </row>
     <row r="20" spans="3:12">
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="24" t="s">
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="I20" s="25"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="21"/>
+      <c r="I20" s="29"/>
+      <c r="J20" s="30"/>
+      <c r="K20" s="25"/>
+      <c r="L20" s="26"/>
     </row>
     <row r="21" spans="3:12">
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="23"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="35"/>
+      <c r="L21" s="36"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="C20:E21"/>
-    <mergeCell ref="F20:G21"/>
-    <mergeCell ref="H20:J21"/>
-    <mergeCell ref="K20:L21"/>
+  <mergeCells count="26">
+    <mergeCell ref="A1:N2"/>
+    <mergeCell ref="C12:G13"/>
+    <mergeCell ref="H12:L13"/>
+    <mergeCell ref="C18:L18"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C17:E17"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K14:L14"/>
     <mergeCell ref="K15:L15"/>
     <mergeCell ref="K16:L16"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="H20:J21"/>
+    <mergeCell ref="K20:L21"/>
     <mergeCell ref="H17:J17"/>
-    <mergeCell ref="H18:J18"/>
     <mergeCell ref="F19:G19"/>
     <mergeCell ref="C19:E19"/>
-    <mergeCell ref="A1:N2"/>
-    <mergeCell ref="C12:G13"/>
-    <mergeCell ref="H12:L13"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -903,30 +931,4 @@
     <brk id="27" max="39" man="1"/>
   </colBreaks>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
@kulasekaran 1. bug number-2(5),6(5),9(3) and 15(3) are solved
</commit_message>
<xml_diff>
--- a/payslipsystem/webroot/templates/pay_slip_template.xlsx
+++ b/payslipsystem/webroot/templates/pay_slip_template.xlsx
@@ -31,59 +31,59 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Date :</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Earnings</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Deductions</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Basic Salary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Insentive</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Medical Allowance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Dearness Allowance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Total Addition</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IT Tax</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PF</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Penalty</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Total Deduction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Net Salary</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>Year :</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Date :</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Earnings</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Deductions</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Basic Salary</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Insentive</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Medical Allowance</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Dearness Allowance</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Total Addition</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>IT Tax</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>PF</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Penalty</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Total Deduction</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Net Salary</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -92,10 +92,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="178" formatCode="#,##0.0;[Red]#,##0.0"/>
-    <numFmt numFmtId="180" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="176" formatCode="#,##0.0;[Red]#,##0.0"/>
+    <numFmt numFmtId="177" formatCode="0;[Red]0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,6 +131,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -262,14 +269,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
@@ -281,68 +285,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -350,29 +297,92 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -676,227 +686,237 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="16384" width="9" style="3"/>
+    <col min="1" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
     </row>
     <row r="2" spans="1:19" ht="15" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
     </row>
     <row r="6" spans="1:19">
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="5"/>
-      <c r="K6" s="3" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="4"/>
+      <c r="K6" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="L6" s="4"/>
+    </row>
+    <row r="8" spans="1:19">
+      <c r="C8" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="10" spans="1:19">
+      <c r="C10" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:19">
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:19">
+      <c r="C12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="5"/>
-    </row>
-    <row r="8" spans="1:19">
-      <c r="C8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="10" spans="1:19">
-      <c r="C10" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="5"/>
-    </row>
-    <row r="11" spans="1:19">
-      <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:19">
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="13"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="8" t="s">
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="14"/>
+    </row>
+    <row r="13" spans="1:19">
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="17"/>
+    </row>
+    <row r="14" spans="1:19">
+      <c r="C14" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="10"/>
-    </row>
-    <row r="13" spans="1:19">
-      <c r="C13" s="11"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="13"/>
-    </row>
-    <row r="14" spans="1:19">
-      <c r="C14" s="14" t="s">
+      <c r="D14" s="24"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="22"/>
+      <c r="H14" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="I14" s="24"/>
+      <c r="J14" s="25"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="22"/>
+    </row>
+    <row r="15" spans="1:19">
+      <c r="C15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="14" t="s">
+      <c r="D15" s="24"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="16"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="18"/>
-    </row>
-    <row r="15" spans="1:19">
-      <c r="C15" s="14" t="s">
+      <c r="I15" s="24"/>
+      <c r="J15" s="25"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="22"/>
+    </row>
+    <row r="16" spans="1:19">
+      <c r="C16" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="22"/>
+      <c r="H16" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="24"/>
+      <c r="J16" s="25"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="22"/>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="C17" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="18"/>
-    </row>
-    <row r="16" spans="1:19">
-      <c r="C16" s="14" t="s">
+      <c r="D17" s="24"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="25"/>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="C18" s="18"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="19"/>
+      <c r="K18" s="19"/>
+      <c r="L18" s="20"/>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="14" t="s">
+      <c r="D19" s="35"/>
+      <c r="E19" s="36"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="18"/>
-    </row>
-    <row r="17" spans="3:12">
-      <c r="C17" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="17"/>
-      <c r="G17" s="18"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="15"/>
-      <c r="J17" s="16"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="16"/>
-    </row>
-    <row r="18" spans="3:12">
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="20"/>
-      <c r="I18" s="20"/>
-      <c r="J18" s="20"/>
-      <c r="K18" s="20"/>
-      <c r="L18" s="21"/>
-    </row>
-    <row r="19" spans="3:12">
-      <c r="C19" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="23"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="14" t="s">
+      <c r="I19" s="24"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="22"/>
+    </row>
+    <row r="20" spans="3:12">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="3:12">
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" s="29"/>
-      <c r="J20" s="30"/>
-      <c r="K20" s="25"/>
-      <c r="L20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="30"/>
+      <c r="L20" s="31"/>
     </row>
     <row r="21" spans="3:12">
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="31"/>
-      <c r="F21" s="31"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="35"/>
-      <c r="L21" s="36"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="10"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="32"/>
+      <c r="L21" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="H20:J21"/>
+    <mergeCell ref="K20:L21"/>
+    <mergeCell ref="H17:J17"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K19:L19"/>
     <mergeCell ref="A1:N2"/>
     <mergeCell ref="C12:G13"/>
     <mergeCell ref="H12:L13"/>
@@ -913,16 +933,6 @@
     <mergeCell ref="H15:J15"/>
     <mergeCell ref="H16:J16"/>
     <mergeCell ref="K14:L14"/>
-    <mergeCell ref="K15:L15"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="H20:J21"/>
-    <mergeCell ref="K20:L21"/>
-    <mergeCell ref="H17:J17"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="C19:E19"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>